<commit_message>
Table finish, table array finish
</commit_message>
<xml_diff>
--- a/Test Brand Data.xlsx
+++ b/Test Brand Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F-SFX\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F-SFX\Desktop\Web Dev Learning\Projects\Projects to post\Verify URL Status Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCCA9698-0D38-41A3-88F7-793B6083DEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237E7393-4534-4A13-96C6-FCFCB4157D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="3060" windowWidth="28800" windowHeight="15435" xr2:uid="{542FE14F-FE1C-42D6-A5A1-0F5A43D6E55B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{542FE14F-FE1C-42D6-A5A1-0F5A43D6E55B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Griffin Art Projects</t>
   </si>
@@ -251,6 +251,15 @@
   </si>
   <si>
     <t>https://www.movestands.com/</t>
+  </si>
+  <si>
+    <t>Brand ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand </t>
+  </si>
+  <si>
+    <t>Brand Url</t>
   </si>
 </sst>
 </file>
@@ -603,407 +612,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740C7145-5B7A-4233-A9D2-E3875A6932C2}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>4103227</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>4103231</v>
+        <v>4103227</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>4106593</v>
+        <v>4103231</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4106597</v>
+        <v>4106593</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4106601</v>
+        <v>4106597</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4106617</v>
+        <v>4106601</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4106619</v>
+        <v>4106617</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>4106627</v>
+        <v>4106619</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4106631</v>
+        <v>4106627</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>4106633</v>
+        <v>4106631</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>4106635</v>
+        <v>4106633</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>4106637</v>
+        <v>4106635</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>4106641</v>
+        <v>4106637</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>4106643</v>
+        <v>4106641</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>4106645</v>
+        <v>4106643</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>4106647</v>
+        <v>4106645</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>4106649</v>
+        <v>4106647</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>4106661</v>
+        <v>4106649</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>4106667</v>
+        <v>4106661</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>4106681</v>
+        <v>4106667</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>4106683</v>
+        <v>4106681</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>4106685</v>
+        <v>4106683</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>4106687</v>
+        <v>4106685</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>4106691</v>
+        <v>4106687</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>4106693</v>
+        <v>4106691</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>4106695</v>
+        <v>4106693</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>4106699</v>
+        <v>4106695</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>4106701</v>
+        <v>4106699</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>4106703</v>
+        <v>4106701</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>4106705</v>
+        <v>4106703</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>4106707</v>
+        <v>4106705</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>4106709</v>
+        <v>4106707</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>4106711</v>
+        <v>4106709</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>4106715</v>
+        <v>4106711</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>4106717</v>
+        <v>4106715</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
+        <v>4106717</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>4103478</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>